<commit_message>
Added a .exist on the username field to give the AOS application ample time to fly down the login screen.
</commit_message>
<xml_diff>
--- a/uft-one-script-against-mockup-aos/Default.xlsx
+++ b/uft-one-script-against-mockup-aos/Default.xlsx
@@ -182,9 +182,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -195,7 +193,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -518,7 +518,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -537,10 +537,10 @@
       </c>
     </row>
     <row>
-      <c s="3" t="s">
+      <c s="2" t="s">
         <v>1</v>
       </c>
-      <c s="2" t="s">
+      <c s="3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Aligned comments in 15.0.2
</commit_message>
<xml_diff>
--- a/uft-one-script-against-mockup-aos/Default.xlsx
+++ b/uft-one-script-against-mockup-aos/Default.xlsx
@@ -182,7 +182,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -193,9 +195,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -537,10 +537,10 @@
       </c>
     </row>
     <row>
-      <c s="2" t="s">
+      <c s="3" t="s">
         <v>1</v>
       </c>
-      <c s="3" t="s">
+      <c s="2" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated screen shot of high rez mockup to include Logout
</commit_message>
<xml_diff>
--- a/uft-one-script-against-mockup-aos/Default.xlsx
+++ b/uft-one-script-against-mockup-aos/Default.xlsx
@@ -182,9 +182,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -195,7 +193,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -537,10 +537,10 @@
       </c>
     </row>
     <row>
-      <c s="3" t="s">
+      <c s="2" t="s">
         <v>1</v>
       </c>
-      <c s="2" t="s">
+      <c s="3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added statement to start the mediaserver Service (viewable via services.msc), which the AI OCR engine requires to have running to properly execute.
</commit_message>
<xml_diff>
--- a/uft-one-script-against-mockup-aos/Default.xlsx
+++ b/uft-one-script-against-mockup-aos/Default.xlsx
@@ -182,7 +182,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -193,9 +195,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -537,10 +537,10 @@
       </c>
     </row>
     <row>
-      <c s="2" t="s">
+      <c s="3" t="s">
         <v>1</v>
       </c>
-      <c s="3" t="s">
+      <c s="2" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Shifted the ExitAction statement in the CompletedScript to be the first line of code.
</commit_message>
<xml_diff>
--- a/uft-one-script-against-mockup-aos/Default.xlsx
+++ b/uft-one-script-against-mockup-aos/Default.xlsx
@@ -182,9 +182,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -195,7 +193,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -537,10 +537,10 @@
       </c>
     </row>
     <row>
-      <c s="3" t="s">
+      <c s="2" t="s">
         <v>1</v>
       </c>
-      <c s="2" t="s">
+      <c s="3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>